<commit_message>
corrected the excel file
</commit_message>
<xml_diff>
--- a/example_outputs_used_in_report/comparative_evaluation_results_used_in_report.xlsx
+++ b/example_outputs_used_in_report/comparative_evaluation_results_used_in_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\GitHub\Augmentent-traditional-search-engine\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\GitHub\LLM-vs-Human-Search-Performance\example_outputs_used_in_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB08B18-6A01-4164-ABD3-6F3608D758E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA5DC09-DCAF-41B7-91D8-F00FF0FBC1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
   <si>
     <t>query</t>
   </si>
@@ -63,180 +63,33 @@
     <t>What is the capital of Italy?</t>
   </si>
   <si>
-    <t>Both results provide information about the capital of Italy, which is Rome. However, Result_A includes multiple queries and results that mention other cities like Milan and Venice, which might confuse the user. Result_B is more focused and consistently mentions Rome as the capital of Italy, making it more straightforward and easier to understand. Therefore, Result_B is better in terms of coherence and relevance.</t>
-  </si>
-  <si>
-    <t>Both sets of results provide information about the capital of Italy, which is Rome. However, Result_A includes multiple queries and results that mention other cities like Milan and Venice, which could potentially confuse the user. Result_B is more focused and consistently mentions Rome as the capital of Italy, providing a more straightforward answer to the query. Therefore, Result_B is likely better in terms of coherence and relevance.</t>
-  </si>
-  <si>
-    <t>Both results provide information about the capital of Italy, which is Rome. However, Result_A includes multiple queries and results that mention other cities like Milan and Venice, which might confuse the user. Result_B is more focused and consistently mentions Rome as the capital of Italy. Therefore, Result_B is more coherent and relevant to the query.</t>
-  </si>
-  <si>
-    <t>Both result sets provide information about the capital of Italy, which is Rome. However, Result_A includes multiple queries and results that mention other cities like Milan and Venice, which might confuse the user. Result_B is more focused and consistently mentions Rome as the capital of Italy. Therefore, Result_B is more coherent and relevant to the query.</t>
-  </si>
-  <si>
-    <t>Both results provide information about the capital of Italy, which is Rome. However, Result_A includes multiple queries and results that mention other cities like Milan and Venice, which could potentially confuse the user. Result_B is more focused and consistently mentions Rome as the capital of Italy without introducing other cities. Therefore, Result_B is more coherent and relevant to the specific query about the capital of Italy.</t>
-  </si>
-  <si>
     <t>Best laptops for students 2023</t>
   </si>
   <si>
-    <t>Result A provides a variety of sources that discuss the best laptops for students in 2023, including specific models and their features. It also includes links to articles and videos that offer detailed reviews and comparisons. Result B, on the other hand, includes a mix of sources that discuss the best laptops for students, but also includes some articles that are less directly related to the query, such as those about laptops for teachers or general laptop recommendations. Overall, Result A is more focused and relevant to the specific query about the best laptops for students in 2023.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that specifically address the query 'Best laptops for students 2023' with multiple articles and reviews from different websites. It includes a mix of general best laptops and those specifically for students, which is useful for the query. Result B, on the other hand, includes some relevant sources but also has entries that are less directly related to the query, such as laptops for teachers and general best laptops for 2023. This makes Result A more focused and relevant to the specific query about student laptops.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that discuss the best laptops for students in 2023, including specific models and their features. It includes links to articles from reputable sources like Digital Trends, T3, and Good Housekeeping. However, some results are slightly off-topic, such as those discussing laptops for 2024. Result B also offers a range of sources but includes some entries that are less directly relevant to the query, such as laptops for teachers and general laptop recommendations. Both results have their strengths, but Result A is slightly more focused on the specific query about the best laptops for students in 2023.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that discuss the best laptops for students in 2023, including specific models and their features. It includes links to articles from reputable sources like Digital Trends, T3, and Good Housekeeping. However, some of the results are slightly off-topic, such as those discussing laptops for 2024 or for different user groups like teachers. Result B, on the other hand, also provides a range of sources but includes more off-topic results, such as laptops for teachers and general laptop recommendations for 2023. Both results have their strengths, but Result A is slightly more focused on the query about the best laptops for students in 2023.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that discuss the best laptops for students in 2023, including specific models and their features. It includes links to articles from reputable sources like Digital Trends, T3, and Good Housekeeping. However, some of the results are slightly off-topic, such as those discussing the best laptops for 2024 or for other specific needs like gaming or lightweight laptops. Result B, on the other hand, is more focused on the specific query about the best laptops for students in 2023. It includes articles from Consumer Reports, Yahoo, and other reputable sources, and it also provides specific recommendations for different needs (e.g., budget, battery life). Overall, Result B is more coherent and relevant to the specific query, but both results have their strengths and weaknesses.</t>
-  </si>
-  <si>
     <t>Details of the Treaty of Versailles</t>
   </si>
   <si>
-    <t>Both results provide detailed information about the Treaty of Versailles, but they differ in the sources and the way the information is presented. Result_A is structured around multiple queries related to the Treaty of Versailles, providing a broader range of sources and perspectives. This makes it more comprehensive but potentially less focused. Result_B, on the other hand, provides a more focused set of results directly addressing the main query, which might make it easier for the user to find specific information quickly. However, it may lack the breadth of perspectives found in Result_A.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured breakdown of different aspects of the Treaty of Versailles, including its history, impact on Germany, key points, and significance. This makes it comprehensive and well-organized. Result B, on the other hand, offers a variety of sources that cover the treaty's details, but it is less structured and more general. Both results are good, but Result A is more methodical and segmented, which can be beneficial for understanding different facets of the treaty. Result B, while still informative, lacks the same level of organization and specificity in addressing different aspects of the treaty.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured breakdown of different aspects of the Treaty of Versailles, including its history, impact on Germany, key points, and significance. This makes it comprehensive and well-organized. Result B, on the other hand, offers a variety of sources that cover the treaty's details but lacks the structured categorization seen in Result A. Both results are good, but Result A is more methodically organized, which can be beneficial for understanding the different facets of the treaty. Result B, while still informative, may require more effort to piece together the full picture due to its less structured presentation.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured breakdown of different aspects of the Treaty of Versailles, including its history, impact on Germany, key points, and significance. This makes it comprehensive and well-organized. Result B, on the other hand, offers a variety of sources but lacks the same level of structured categorization. Both results are good, but Result A is more methodical and easier to follow, which could be beneficial for someone looking for detailed and organized information.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured breakdown of different aspects of the Treaty of Versailles, including its history, impact on Germany, key points, and significance. This makes it more comprehensive and easier to navigate for specific details. Result B, while also providing relevant information, is less structured and mixes different aspects of the treaty in a single list. This can make it harder to find specific information quickly. Both results are good, but Result A is more organized and thorough in covering various facets of the Treaty of Versailles.</t>
-  </si>
-  <si>
     <t>Results of the 2022 FIFA World Cup final</t>
   </si>
   <si>
-    <t>Result_A provides a structured breakdown of different aspects of the 2022 FIFA World Cup final, including the winner, score, highlights, and best player. This makes it more comprehensive and easier to follow. Result_B, on the other hand, is a list of various articles related to the World Cup final but lacks the structured approach seen in Result_A. Result_A is better because it directly addresses multiple facets of the query in a more organized manner.</t>
-  </si>
-  <si>
-    <t>Result_A provides a structured breakdown of different aspects of the 2022 FIFA World Cup final, including the winner, score, highlights, and best player. This makes it more comprehensive and easier to follow. Result_B, while also providing relevant information, is less structured and includes some links that are not directly related to the final match itself. Result_A is better because it directly addresses various facets of the final match in a more organized manner.</t>
-  </si>
-  <si>
-    <t>Result_A provides a structured breakdown of different aspects of the 2022 FIFA World Cup final, including the winner, score, highlights, and best player. This makes it more comprehensive and easier to follow. Result_B, while also providing relevant information, is less structured and includes some links that are not directly related to the final match. Therefore, Result_A is more focused and organized, making it potentially better for someone looking for detailed information about the final.</t>
-  </si>
-  <si>
-    <t>Result A is structured as a series of queries and their corresponding results, which makes it more organized and easier to follow. It provides multiple sources for each query, ensuring a comprehensive answer. Result B, on the other hand, is a list of individual results without clear separation of different queries, which can make it harder to discern the specific information related to the original query. Result A is better because it directly addresses the query with multiple relevant sources and clear organization.</t>
-  </si>
-  <si>
-    <t>Result_A provides a structured breakdown of multiple queries related to the 2022 FIFA World Cup final, including the winner, score, highlights, and best player. This makes it more comprehensive and targeted. Result_B, on the other hand, offers a more general collection of links and information about the final but lacks the structured approach seen in Result_A. Result_A is better because it directly addresses various aspects of the query in a more organized manner.</t>
-  </si>
-  <si>
     <t>How does blockchain technology work?</t>
   </si>
   <si>
-    <t>Result A provides multiple sets of results for different variations of the query, which can be beneficial for covering a broader range of information. However, this can also lead to redundancy and make it harder to find a concise answer. Result B, on the other hand, offers a single set of results that are more streamlined and focused. This makes it easier to navigate but might miss out on some variations of the query. Both results include reputable sources and cover the basics of blockchain technology, but Result A's approach might be more comprehensive due to the multiple query variations.</t>
-  </si>
-  <si>
-    <t>Result A provides multiple sets of results for different variations of the query, which can be beneficial for understanding the topic from various perspectives. It includes a mix of sources like Wikipedia, Investopedia, and freeCodeCamp, which are known for their detailed explanations. Result B, on the other hand, offers a single set of results but from a diverse range of sources including The Economist, CoinDesk, and Deloitte. Both results are good, but Result A might be slightly better due to its broader approach in addressing different query variations, which can provide a more comprehensive understanding of blockchain technology.</t>
-  </si>
-  <si>
-    <t>Result A provides multiple sets of results for different but related queries about blockchain technology, which can be useful for a comprehensive understanding. However, it may also introduce redundancy as some sources are repeated across different queries. Result B, on the other hand, offers a single set of results directly addressing the query, which makes it more straightforward but potentially less comprehensive. Both results include reputable sources, but Result A's approach might be more thorough due to the variety of queries it covers.</t>
-  </si>
-  <si>
-    <t>Result A provides multiple sets of results for different variations of the query, which can be beneficial for understanding the topic from various angles. This approach ensures that the user gets a comprehensive view of blockchain technology. However, it might be slightly overwhelming due to the repetition of similar information. Result B, on the other hand, offers a single set of results that are diverse and cover different aspects of blockchain technology. This makes it more straightforward and easier to digest. Both results are good, but Result B might be slightly better due to its simplicity and directness.</t>
-  </si>
-  <si>
-    <t>Result A provides multiple sets of results for different variations of the query, which can be beneficial for covering a broader range of information. However, this can also lead to redundancy as some sources are repeated across different queries. Result B, on the other hand, offers a single set of results that are diverse and cover various aspects of blockchain technology. This makes Result B more streamlined and easier to follow. Both results include reputable sources, but Result B is more concise and avoids repetition, making it potentially more effective for a user seeking a clear and comprehensive answer.</t>
-  </si>
-  <si>
     <t>What are the pros and cons of keto diet?</t>
   </si>
   <si>
-    <t>Result A provides a more structured and categorized approach to the query by breaking down the information into different sub-queries such as 'pros and cons of keto diet,' 'benefits of ketogenic diet,' 'risks of keto diet,' etc. This makes it easier to find specific information. However, it may require the user to look through multiple links to get a comprehensive understanding. Result B, on the other hand, directly addresses the pros and cons of the keto diet in a more straightforward manner, making it easier for the user to get a quick overview. Both results are good, but Result B is more focused on the specific query and provides a more direct answer.</t>
-  </si>
-  <si>
-    <t>Result A provides a broader range of sources and covers various aspects of the keto diet, including its benefits, risks, and comparisons with other diets. However, it does not directly address the pros and cons in a single, cohesive manner. Result B, on the other hand, directly addresses the pros and cons of the keto diet with specific articles focused on this topic. This makes Result B more directly relevant to the query. Both results have their strengths: A offers a wider context, while B is more focused on the specific query.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that discuss the pros and cons of the keto diet, but it also includes results that are not directly related to the query, such as keto meal plans and success stories. This dilutes the focus on the pros and cons. Result B, on the other hand, is more focused on the specific query about the pros and cons of the keto diet, providing multiple sources that directly address this topic. Therefore, Result B is more targeted and relevant to the query. Both results offer valuable information, but Result B is more coherent and complete in addressing the specific question asked.</t>
-  </si>
-  <si>
-    <t>Result A provides a variety of sources that discuss the pros and cons of the keto diet, including its benefits, risks, and comparisons to other diets. However, it does not directly address the pros and cons in a single, cohesive manner. Result B, on the other hand, includes sources that specifically focus on the pros and cons of the keto diet, making it more directly relevant to the query. Both results have their strengths, but Result B is more focused on the specific query about the pros and cons of the keto diet.</t>
-  </si>
-  <si>
-    <t>Result A provides a broader range of sources and covers various aspects of the keto diet, including its benefits, risks, and comparisons with other diets. However, it does not directly address the pros and cons in a single, cohesive manner. Result B, on the other hand, directly addresses the pros and cons of the keto diet with specific articles focused on this topic. This makes Result B more directly relevant to the query. Both results have their strengths, but Result B is more focused on the specific query about the pros and cons of the keto diet.</t>
-  </si>
-  <si>
     <t>Impact of Brexit on UK economy</t>
   </si>
   <si>
-    <t>Result A provides a more structured and organized set of results, with each query and its corresponding results clearly delineated. This makes it easier to follow and understand the context of each result. Result B, on the other hand, presents a single list of results without clear separation of different queries, which can make it harder to discern the specific context of each result. Additionally, Result A includes multiple sources for each query, offering a broader perspective, while Result B has fewer sources but includes some unique articles not found in Result A. Both results are good, but Result A is slightly better in terms of organization and breadth of sources.</t>
-  </si>
-  <si>
-    <t>Both result sets provide a variety of sources discussing the impact of Brexit on the UK economy. However, there are some differences in the breadth and depth of the information provided. Result_A includes multiple queries and their corresponding results, which might offer a broader perspective but can also be repetitive. Result_B, on the other hand, provides a more concise list of sources directly addressing the query. Result_B also includes a mix of sources from different perspectives, which might provide a more balanced view. Overall, Result_B seems to be more focused and less repetitive, making it potentially more useful for someone looking for a comprehensive yet concise overview.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured response with multiple queries and their corresponding results, which gives a broader perspective on the impact of Brexit on the UK economy. It includes various sources like BBC, Wikipedia, and LSE, which are reputable and provide a comprehensive view. Result B, on the other hand, presents a single list of articles without breaking them down by specific queries. While it also includes reputable sources like The Guardian, Financial Times, and BBC, it lacks the structured approach seen in Result A. This makes Result A more organized and potentially more useful for someone looking for detailed information on different aspects of the Brexit impact.</t>
-  </si>
-  <si>
-    <t>Result A provides a structured response with multiple queries and corresponding results, which gives a broader perspective on the impact of Brexit on the UK economy. It includes various sources like BBC, Wikipedia, and LSE, which are reputable and provide detailed insights. Result B, on the other hand, offers a more concise list of articles but lacks the structured approach seen in Result A. While both results include relevant and credible sources, Result A's structured format and variety of sources make it more comprehensive and easier to follow.</t>
-  </si>
-  <si>
-    <t>Both result sets provide a variety of sources discussing the impact of Brexit on the UK economy. However, there are some differences in the breadth and depth of the information provided. Result_A includes multiple queries with a range of sources, which might offer a more comprehensive view but could also be seen as repetitive. Result_B, on the other hand, provides a more concise set of results but includes some unique sources not found in Result_A. Overall, Result_A might be better for someone looking for a broader range of perspectives, while Result_B could be more suitable for someone seeking a more focused set of high-quality sources.</t>
-  </si>
-  <si>
     <t>Which is better for home use: solar panels or wind turbines?</t>
   </si>
   <si>
-    <t>Result A provides a more structured and detailed comparison between solar panels and wind turbines for home use. It includes multiple queries that address various aspects such as advantages, disadvantages, costs, and specific use cases. This makes it more comprehensive and informative. Result B, while also providing useful information, is less structured and does not cover as many specific aspects of the comparison. Result A is better for someone looking for a detailed and thorough comparison, while Result B is more general and less detailed.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and detailed comparison between solar panels and wind turbines for home use. It includes multiple queries that address various aspects such as advantages, disadvantages, costs, and specific use cases. This makes it more comprehensive and informative. Result B, on the other hand, offers a more general comparison with fewer specific details and less structured information. While both results are useful, Result A is more thorough and better organized, making it more suitable for someone looking for an in-depth comparison.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and detailed comparison between solar panels and wind turbines for home use. It includes multiple queries that address various aspects such as advantages, disadvantages, costs, and specific use cases. This makes it more comprehensive and informative. Result B, on the other hand, offers a more general comparison with fewer specific details and sources. While it covers the main points, it lacks the depth and variety of perspectives found in Result A. Therefore, Result A is likely to be more useful for someone looking for a thorough understanding of the topic.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and detailed set of results, breaking down the information into specific queries related to solar panels and wind turbines. This includes costs, advantages, disadvantages, and a direct comparison between the two. This makes it easier for the user to find specific information. Result B, on the other hand, offers a more general comparison between solar panels and wind turbines without breaking down the information into specific sub-queries. While both sets of results are useful, Result A is more comprehensive and organized, making it potentially more useful for someone looking to make an informed decision between solar panels and wind turbines for home use.</t>
-  </si>
-  <si>
     <t>Is artificial intelligence beneficial to society?</t>
   </si>
   <si>
-    <t>Result A provides a more structured and detailed set of responses, with multiple queries and corresponding results that directly address the benefits and positive impacts of artificial intelligence on society. This makes it more comprehensive and targeted towards the query. Result B, while also providing relevant information, is less structured and includes a broader range of topics, some of which are not directly focused on the benefits of AI to society. This makes Result A more coherent and complete in addressing the specific query.</t>
-  </si>
-  <si>
-    <t>Result_A provides a structured list of search queries and their corresponding results, which are directly related to the benefits and positive impacts of artificial intelligence on society. This makes it easier to find specific information related to the query. Result_B, on the other hand, offers a more general list of articles that discuss AI's impact on society, but it is less structured and some articles are not directly focused on the benefits of AI. Therefore, Result_A is more targeted and relevant to the query, while Result_B provides a broader perspective but may include less relevant information.</t>
-  </si>
-  <si>
-    <t>Result_A provides multiple sets of search results based on different queries related to the benefits of artificial intelligence to society. This approach ensures a broad coverage of the topic from various angles, such as societal development, positive impacts, and specific advantages. Result_B, on the other hand, offers a single set of search results that are more general and include a mix of articles discussing both the benefits and potential risks of AI. While Result_A is more focused and comprehensive in addressing the specific query about the benefits of AI, Result_B provides a broader context, which might be useful but is less targeted. Therefore, Result_A is better suited for the specific query about the benefits of AI to society.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and detailed set of results, with multiple queries that are closely related to the original question about the benefits of artificial intelligence to society. Each query in Result A is followed by multiple sources that discuss various aspects of AI's positive impact. This makes Result A more comprehensive and targeted. Result B, on the other hand, offers a single set of results that are somewhat relevant but less focused on the specific query. Result B includes a mix of articles that discuss AI's impact on society, but it also includes sources that touch on potential risks and ethical dilemmas, which are not directly aligned with the query about benefits. Therefore, Result A is better in terms of relevance and completeness, while both results are fairly coherent.</t>
-  </si>
-  <si>
-    <t>Result_A provides a structured list of search queries and their corresponding results, which are directly related to the benefits and positive impacts of artificial intelligence on society. This makes it easier to see the specific aspects of AI's benefits being addressed. Result_B, on the other hand, offers a more general collection of articles that discuss AI's impact on society, but it is less structured and more varied in focus. Result_A is more targeted and organized, making it potentially more useful for someone specifically looking for the benefits of AI to society. However, Result_B includes a broader range of perspectives, which could be beneficial for a more comprehensive understanding of AI's societal impact.</t>
-  </si>
-  <si>
     <t>What is the best way to achieve a work-life balance?</t>
   </si>
   <si>
-    <t>Result A provides a more structured and comprehensive set of results by breaking down the query into multiple sub-queries, each addressing different aspects of work-life balance. This approach ensures a broader coverage of the topic, including tips, strategies, importance, and impact on mental health. Result B, on the other hand, offers a single list of articles that are relevant but less structured. While both sets of results are useful, Result A is likely to be more helpful for someone looking for a detailed and multifaceted understanding of work-life balance.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and comprehensive set of results by breaking down the query into multiple sub-queries, each addressing different aspects of work-life balance. This approach ensures a broader coverage of the topic, including tips, strategies, importance, and impact on mental health. Result B, on the other hand, offers a single list of articles that are relevant but less structured. While both sets of results are useful, Result A is likely to be more helpful for someone looking for a detailed and multifaceted understanding of work-life balance. Result B is more straightforward but may miss out on some nuanced aspects covered in Result A.</t>
-  </si>
-  <si>
-    <t>Result_A provides a more structured and comprehensive set of results, with multiple queries and corresponding results that cover various aspects of work-life balance, such as best practices, effective strategies, and the importance of work-life balance. This makes it more thorough and potentially more useful for someone looking for detailed information. Result_B, on the other hand, offers a single set of results that are also relevant but less diverse in terms of the queries addressed. While both sets are good, Result_A is more detailed and covers a broader range of topics related to work-life balance.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and comprehensive set of results by breaking down the query into multiple sub-queries, each addressing different aspects of work-life balance. This approach ensures a broader coverage of the topic, including tips, strategies, importance, and impact on mental health. Result B, on the other hand, offers a more straightforward list of articles without breaking down the query into sub-queries. While Result B is simpler and easier to navigate, it may lack the depth and variety of perspectives found in Result A. Both results are good, but Result A is more thorough and detailed, making it potentially more useful for someone seeking a comprehensive understanding of work-life balance.</t>
-  </si>
-  <si>
-    <t>Result A provides a more structured and comprehensive set of results, with multiple queries and corresponding results that cover various aspects of work-life balance, such as best practices, effective strategies, and the importance of work-life balance. This makes it more thorough and potentially more useful for someone seeking detailed information. Result B, on the other hand, offers a single set of results that are also relevant but less varied in terms of the angles they cover. Result A is likely better for someone looking for a wide range of tips and strategies, while Result B is more straightforward and concise.</t>
-  </si>
-  <si>
     <t>query_</t>
   </si>
   <si>
@@ -283,6 +136,147 @@
   </si>
   <si>
     <t>OVERALL DIFF</t>
+  </si>
+  <si>
+    <t>Both results provide a clear answer to the query, stating that Rome is the capital of Italy. However, there are some differences in the sources and additional information provided. Result_A includes more historical context and mentions other major cities in Italy, while Result_B focuses more on geographical and administrative details. Both results list relevant sources, but Result_A provides a broader range of information, including the economic significance of Milan. Result_B, on the other hand, includes a source specifically aimed at children, which might be less relevant for a general audience. Overall, both results are good, but Result_A offers a slightly more comprehensive view.</t>
+  </si>
+  <si>
+    <t>Both results provide a clear answer to the query, stating that Rome is the capital of Italy. However, there are some differences in the sources and additional information provided. Result A includes more sources and additional context about other important cities in Italy, while Result B focuses more on the historical and geographical context of Rome. Both results are good, but Result A might be slightly better due to its broader range of sources and additional context about other cities.</t>
+  </si>
+  <si>
+    <t>Both results provide a clear answer to the query, stating that the capital of Italy is Rome. However, there are some differences in the sources cited and the additional information provided. Result A includes more sources and provides a broader context, mentioning other important cities in Italy and the historical context of Rome becoming the capital. Result B, on the other hand, focuses more on the geographical and historical significance of Rome. Both results are good, but Result A is slightly more comprehensive and detailed, which could make it more useful for someone seeking in-depth information.</t>
+  </si>
+  <si>
+    <t>Both results provide a clear answer to the query, stating that Rome is the capital of Italy. However, there are some differences in the sources and additional information provided. Result_A includes more sources and additional context about other important cities in Italy, which might be seen as extra but not directly relevant to the query. Result_B focuses more on Rome and provides sources that are more directly related to the capital status of Rome. Both results are good, but Result_B is slightly more focused on the query without adding potentially extraneous information.</t>
+  </si>
+  <si>
+    <t>Both results provide a clear answer to the query, stating that the capital of Italy is Rome. However, there are some differences in the sources cited and the additional information provided. Result_A includes more sources and provides a broader context, mentioning other major cities in Italy and the historical context of Rome becoming the capital. Result_B, on the other hand, focuses more on the geographical and historical significance of Rome. Both results are good, but Result_A offers a slightly more comprehensive view by including more sources and additional context about other cities and historical facts.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of sources that recommend the best laptops for students in 2023. However, there are some differences in the presentation and content. Result A includes a mix of sources, including a YouTube video and a site focused on lightweight laptops, which may offer a broader perspective. Result B, on the other hand, includes sources that are more focused on specific needs, such as battery life and screen size, and also includes a source for teachers, which may not be directly relevant to students. Result A might be considered better for its broader range of sources and more direct focus on student needs.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of recommended laptops for students in 2023, but they differ in their sources and presentation. Result A includes a mix of articles and a YouTube video, while Result B focuses solely on articles from well-known tech and consumer review sites. Result A is more diverse in its sources, which could be beneficial for users looking for different types of content (e.g., video reviews). However, Result B is more focused on written articles, which might be more reliable and easier to reference. Both results are good, but Result A might be slightly better for users who prefer a variety of content types.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of sources that recommend the best laptops for students in 2023. However, there are some differences in the presentation and content. Result A includes a mix of articles and a YouTube video, while Result B focuses solely on articles. Result A also provides a brief description of each source, which helps in understanding the context better. Result B, on the other hand, includes a mix of sources that are not all directly related to the query (e.g., laptops for teachers in 2024). This makes Result A more focused and relevant to the query. Additionally, Result A is more coherent and logically structured, making it easier to follow.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of sources that recommend the best laptops for students in 2023. However, there are some differences in the presentation and content. Result A includes a mix of sources, including a YouTube video and a site focused on lightweight laptops, which might be more engaging for some users. Result B, on the other hand, includes more traditional tech review sites and a broader range of criteria, such as battery life and screen size. Result A might be better for users looking for a quick overview with diverse media, while Result B offers more detailed and specific recommendations. Both results are good, but they cater to slightly different needs and preferences.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of sources that recommend the best laptops for students in 2023. However, there are some differences in their presentation and content. Result A includes a mix of sources, including a YouTube video and a site focused on lightweight laptops, which may not be directly relevant to all students. Result B, on the other hand, focuses more on written articles from well-known tech and consumer review sites, which might be more reliable and easier to reference. Result A also includes a mix of languages, which could be confusing for some users. Overall, Result B seems to be more focused and relevant to the query.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of websites that offer detailed information about the Treaty of Versailles. Result A includes a brief description of each source and its relevance to the topic, while Result B also provides descriptions but focuses more on the historical context and the specific aspects covered by each source. Result A is slightly more detailed in its descriptions, which might make it more useful for someone looking for a comprehensive understanding. However, both results are good and provide valuable resources.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of websites that offer detailed information about the Treaty of Versailles. Result A includes a brief description of each source and its relevance to the topic, while Result B also provides descriptions but focuses more on the historical context and specific aspects of the treaty. Result A is slightly more structured and detailed in its descriptions, which might make it easier for the user to understand the relevance of each source. However, both results are quite comprehensive and relevant to the query.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of websites that offer detailed information about the Treaty of Versailles. Result A is more detailed in its descriptions and provides a more comprehensive overview of what each source covers. It also includes a brief explanation of the historical context and significance of the treaty. Result B, while also providing relevant sources, is less detailed in its descriptions and does not offer as much context about the treaty itself. Therefore, Result A could be considered better due to its thoroughness and the additional context it provides.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of websites that offer detailed information about the Treaty of Versailles. Result A includes a brief description of each source and its relevance to the topic, while Result B also provides descriptions but focuses more on the historical context and the implications of the treaty. Result A is slightly more detailed in its descriptions, which might make it more useful for someone looking for a comprehensive understanding. However, both results are good and provide valuable resources. Result A might be considered better due to its slightly more detailed descriptions and the inclusion of the impact of the treaty on the rise of National Socialism and World War II.</t>
+  </si>
+  <si>
+    <t>Both results provide a list of websites that offer detailed information about the Treaty of Versailles. Result A is more detailed in its descriptions and provides a more comprehensive overview of what each source covers. Result B, while also providing relevant sources, is slightly less detailed in its descriptions. Result A might be considered better due to its thoroughness and the additional context it provides for each source, which can help users better understand what to expect from each link.</t>
+  </si>
+  <si>
+    <t>Both results provide detailed information about the 2022 FIFA World Cup final, including the teams involved, the outcome, and key moments. However, Result_A offers a more narrative and descriptive account, including specific details about the match and its significance, while Result_B is more concise and structured, focusing on the essential facts. Result_A might be better for readers looking for a more engaging and comprehensive story, whereas Result_B is more suitable for those seeking quick and clear information.</t>
+  </si>
+  <si>
+    <t>Both results provide detailed information about the 2022 FIFA World Cup final, including the teams involved, the outcome, and key moments. However, Result_A offers a more narrative and descriptive account, including specific details about the match and its significance, while Result_B is more concise and structured, focusing on the essential facts. Result_A might be better for readers looking for a more comprehensive and engaging summary, whereas Result_B is more suitable for those seeking quick and straightforward information.</t>
+  </si>
+  <si>
+    <t>Both results provide detailed information about the 2022 FIFA World Cup final, including the teams involved, the outcome, and key moments. However, Result_A offers a more narrative and descriptive account, including multiple sources and additional context about the match's excitement and key players. Result_B is more concise and structured, providing clear bullet points that directly address the query. Result_A might be better for readers looking for a more comprehensive and engaging read, while Result_B is more straightforward and easier to scan for specific details.</t>
+  </si>
+  <si>
+    <t>Both results provide detailed information about the 2022 FIFA World Cup final, including the teams involved, the outcome, and key moments. However, there are some differences in presentation and detail. Result_A provides a more narrative style with multiple sources and additional context about the match, while Result_B is more structured and concise, listing key points directly. Result_A might be better for readers looking for a more comprehensive and engaging read, whereas Result_B is more straightforward and to the point. Both are good, but their effectiveness depends on the reader's preference for detail versus brevity.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of how blockchain technology works, but they differ in structure and detail. Result A focuses on summarizing information from various sources and provides URLs for further reading. It is more structured and easier to follow, with clear bullet points and a logical flow. Result B, on the other hand, offers a more detailed explanation of the blockchain's functionality and includes specific examples of its applications. However, it is slightly less structured and can be harder to follow due to its dense text. Overall, Result A is more coherent and easier to read, while Result B is more detailed and thorough.</t>
+  </si>
+  <si>
+    <t>Both results provide a detailed explanation of how blockchain technology works, but they differ in structure and depth. Result A focuses more on listing and summarizing various sources, providing a broad overview of blockchain technology from different perspectives. It includes URLs for further reading, which can be useful for users seeking more in-depth information. Result B, on the other hand, offers a more structured and detailed explanation of blockchain technology, breaking down the concept into specific points and providing a more comprehensive answer. It also includes URLs but integrates them more seamlessly into the explanation. Overall, Result B might be considered better due to its structured approach and detailed explanation, making it easier for readers to understand the concept of blockchain technology.</t>
+  </si>
+  <si>
+    <t>Both results aim to explain how blockchain technology works by providing definitions, explanations, and relevant sources. Result A focuses more on listing and summarizing various sources, while Result B provides a more structured explanation of blockchain technology, followed by a list of sources. Result B is slightly more detailed in explaining the steps and mechanisms involved in blockchain technology, making it potentially more informative for someone seeking a comprehensive understanding. However, both results are coherent and relevant, with Result B having a slight edge in completeness due to its structured approach.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of how blockchain technology works, but they differ in structure and detail. Result_A lists five sources and summarizes the key points from each, providing a broad range of perspectives. Result_B, on the other hand, synthesizes information from multiple sources into a more cohesive narrative before listing the sources at the end. Result_A might be better for someone looking for a quick overview with direct links to more detailed explanations, while Result_B offers a more integrated explanation, which could be more useful for someone seeking a deeper understanding in a single read. Both results are good, but they serve slightly different purposes.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of how blockchain technology works, but they differ in structure and detail. Result A focuses more on listing and summarizing various sources, providing a broad range of perspectives. It includes URLs for further reading, which can be useful for users seeking more in-depth information. Result B, on the other hand, offers a more detailed explanation within the response itself, breaking down the concept into several key points and then listing sources at the end. This makes Result B more self-contained and potentially more useful for someone looking for a quick yet thorough understanding without needing to visit external links. However, Result A might be better for users who prefer to explore multiple sources on their own.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the pros and cons of the keto diet, but they differ in structure and detail. Result_A is more structured, listing specific sources for each point and providing a broader range of information, including success stories and comparisons with other diets. Result_B, while also detailed, focuses more on summarizing the pros and cons from various sources without the additional context provided in Result_A. Result_A could be considered better due to its structured approach and additional context, making it more informative and easier to follow.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the pros and cons of the keto diet, but they differ in structure and detail. Result_A is more structured, listing specific sources for each point and providing a broader range of information, including success stories and comparisons with other diets. Result_B, while also detailed, focuses more on summarizing the pros and cons from various sources without the additional context provided in Result_A. Result_A could be considered better due to its structured approach and additional context, which may help users make a more informed decision.</t>
+  </si>
+  <si>
+    <t>Both results provide a detailed overview of the pros and cons of the keto diet, but they differ in structure and depth. Result_A is more structured, listing pros and cons separately and providing additional sections like success stories and comparisons with other diets. This makes it more comprehensive and easier to follow. Result_B, while also detailed, is less structured and mixes pros and cons within the same points, which might make it slightly harder to parse. However, both results cite reputable sources and cover the essential aspects of the keto diet. Result_A could be considered better due to its structured approach and additional sections that provide a broader perspective.</t>
+  </si>
+  <si>
+    <t>Both results provide a detailed overview of the pros and cons of the keto diet, but they differ in structure and depth. Result_A is more structured, listing pros and cons separately and providing additional sections like success stories and comparisons with other diets. This makes it more comprehensive and easier to follow. Result_B, while also detailed, is less structured and mixes pros and cons within the same points, which might make it slightly harder to follow. However, both results cite reputable sources and cover the essential aspects of the keto diet. Result_A could be considered better due to its structured approach and additional information, but both are good in terms of content quality.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the impact of Brexit on the UK economy, but they differ in their presentation and sources. Result_A offers a more structured and detailed summary of each source, including links and brief descriptions, which makes it easier to follow and understand. Result_B, while also providing relevant sources, is less structured and includes fewer details about each source. Result_A is more coherent and complete due to its structured format and detailed summaries, making it easier for the reader to grasp the information quickly.</t>
+  </si>
+  <si>
+    <t>Both results provide valuable information on the impact of Brexit on the UK economy, but they differ in structure and content. Result_A offers a more structured and detailed list of sources, including summaries and links to articles from reputable sources like BBC News, Wikipedia, and Financial Times. This makes it easier for the reader to understand the context and access further information. Result_B, on the other hand, provides a more concise list of sources with brief descriptions and links, but it lacks the detailed summaries found in Result_A. While both results are good, Result_A is more comprehensive and user-friendly due to its detailed summaries and structured format.</t>
+  </si>
+  <si>
+    <t>Both results provide valuable information on the impact of Brexit on the UK economy, but they differ in structure and content. Result_A offers a more structured and detailed list of sources, including summaries and links, which makes it easier to navigate and understand. Result_B, while also providing relevant sources, is less structured and includes fewer details about each source. Result_A is likely better for users seeking a comprehensive overview, while Result_B might be more suitable for those looking for specific insights quickly.</t>
+  </si>
+  <si>
+    <t>Both results provide valuable information on the impact of Brexit on the UK economy, but they differ in structure and content. Result_A offers a more structured and detailed list of sources, including summaries and links, which makes it easier to follow and understand. It also includes multiple sources from BBC News, Wikipedia, and Financial Times, providing a broad perspective. Result_B, on the other hand, provides a more concise list of sources with brief descriptions and links. While it includes reputable sources like The Guardian and Financial Times, it lacks the detailed summaries found in Result_A. Overall, Result_A is more comprehensive and coherent, making it a better response to the query.</t>
+  </si>
+  <si>
+    <t>Both results provide valuable information regarding the impact of Brexit on the UK economy, but they differ in structure and content. Result A offers a more structured and detailed list of sources, including summaries and links to articles from reputable sources like BBC News, Wikipedia, and Financial Times. This makes it easier for the reader to understand the context and access further information. Result B, on the other hand, provides a more concise list of sources with brief descriptions and links, but it lacks the detailed summaries found in Result A. While both results are good, Result A is more comprehensive and user-friendly due to its detailed summaries and structured format.</t>
+  </si>
+  <si>
+    <t>Both results aim to address the query about whether solar panels or wind turbines are better for home use. Result A provides a more structured and detailed comparison, including multiple sources and specific aspects such as costs, benefits, and environmental impact. It also includes links to various articles for further reading. Result B, while also informative, is less detailed and structured. It provides fewer sources and less comprehensive information. Result A is likely better because it offers a more thorough analysis and a broader range of perspectives, making it more useful for someone trying to make an informed decision.</t>
+  </si>
+  <si>
+    <t>Both results aim to address the query about whether solar panels or wind turbines are better for home use. Result_A provides a more structured and detailed comparison, including multiple sources and specific articles that discuss various aspects such as costs, benefits, and environmental impact. It also includes a summary that highlights the factors to consider when making a decision. Result_B, on the other hand, is more concise and focuses on summarizing key points from a few sources. It also lists the top five relevant websites for further reading. While both results are informative, Result_A offers a more comprehensive and detailed analysis, making it potentially more useful for someone looking for an in-depth understanding. Result_B is more straightforward and easier to read but lacks the depth and breadth of Result_A.</t>
+  </si>
+  <si>
+    <t>Both results provide a comparison between solar panels and wind turbines for home use, but they differ in their approach and depth. Result A offers a more structured and detailed analysis, including multiple sources and specific articles that cover various aspects such as costs, benefits, and environmental impact. It also provides a balanced view by listing both the pros and cons of each option. Result B, on the other hand, is more concise and focuses on summarizing key points from a few sources. While it is easier to read, it lacks the depth and breadth of information found in Result A. Therefore, Result A is more comprehensive and informative, making it a better response overall.</t>
+  </si>
+  <si>
+    <t>Both results aim to address the query about whether solar panels or wind turbines are better for home use. Result_A provides a more structured and detailed comparison, including multiple sources and specific aspects such as costs, benefits, and environmental impact. It also includes links to various articles and guides, making it a comprehensive answer. Result_B, while also informative, is less detailed and structured. It provides fewer sources and less in-depth analysis, focusing more on general statements about the efficiency and cost-effectiveness of both options. Overall, Result_A is more thorough and well-rounded, making it a better response to the query.</t>
+  </si>
+  <si>
+    <t>Both results aim to address the query about whether solar panels or wind turbines are better for home use. Result_A provides a more structured and detailed comparison, including multiple sources and specific articles that discuss various aspects such as costs, benefits, and environmental impact. It also includes a summary that highlights the factors to consider when making a decision. Result_B, on the other hand, is more concise and focuses on summarizing key points from a few sources. It also lists the top five relevant websites for further reading. While both results are informative, Result_A offers a more comprehensive and detailed analysis, making it potentially more useful for someone looking for an in-depth understanding. Result_B is more straightforward and easier to read but lacks the depth and breadth of information found in Result_A.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the benefits of artificial intelligence to society, but they differ in structure and depth. Result_A is more detailed and structured, providing specific examples and sources that highlight the positive impacts of AI. It also includes a variety of sources that cover different aspects of AI's benefits. Result_B, while also providing relevant information, is less detailed and structured. It lists sources and briefly mentions the benefits but does not delve as deeply into specific examples or provide as much context. Therefore, Result_A is more thorough and informative, making it a better response overall.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the benefits of artificial intelligence to society, but they differ in structure and depth. Result_A is more detailed and structured, providing specific examples and sources that highlight the positive impacts of AI. It also includes a variety of sources that cover different aspects of AI's benefits. Result_B, while also providing relevant information, is less detailed and structured. It lists sources and briefly mentions the benefits but lacks the depth and specific examples found in Result_A. Therefore, Result_A is more thorough and informative, making it a better response overall.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the benefits of artificial intelligence to society, but they differ in structure and detail. Result_A is more structured and detailed, providing specific examples and sources that highlight the positive impacts of AI. It also includes a variety of sources that cover different aspects of AI's benefits. Result_B, while also providing relevant information, is less detailed and structured. It lists sources and briefly mentions the benefits but does not delve into specific examples as thoroughly as Result_A. Therefore, Result_A could be considered better due to its detailed and structured approach, which makes it more informative and easier to follow.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the benefits of artificial intelligence to society, but they differ in structure and depth. Result_A is more detailed and structured, providing specific examples and sources that highlight the positive impacts of AI. It also includes a variety of sources, which adds to its credibility. Result_B, while also informative, is less detailed and structured, and it does not provide as many specific examples or sources. Result_A is better because it offers a more thorough and well-organized response, making it easier for the reader to understand the benefits of AI.</t>
+  </si>
+  <si>
+    <t>Both results provide a comprehensive overview of the benefits of artificial intelligence to society, but they differ in structure and depth. Result_A is more detailed and structured, providing specific examples and sources that highlight the positive impacts of AI. It also includes a variety of sources that cover different aspects of AI's benefits. Result_B, while also informative, is less detailed and more general in its approach. It provides fewer specific examples and sources, which might make it less compelling. Overall, Result_A is more thorough and well-organized, making it a better response to the query.</t>
+  </si>
+  <si>
+    <t>Both results provide comprehensive answers to the query about achieving work-life balance, but they differ in structure and detail. Result_A is more structured, breaking down the information into specific categories and providing detailed explanations for each. It also includes direct links to relevant sources. Result_B, while also detailed, is less structured and more narrative in its approach. It provides practical tips but does not categorize them as clearly as Result_A. Result_A might be considered better for someone looking for a more organized and segmented approach, while Result_B is good for those who prefer a more fluid narrative. Both are good, but Result_A edges out slightly due to its structured format and clear categorization.</t>
+  </si>
+  <si>
+    <t>Both results provide comprehensive answers to the query about achieving work-life balance, but they differ in structure and detail. Result_A is more structured, breaking down the information into specific categories and providing detailed explanations for each. It also includes direct links to relevant sources. Result_B, while also detailed, is less structured and more narrative in its approach. It provides practical tips but does not categorize them as clearly as Result_A. Result_A might be considered better for its structured approach and detailed breakdown, making it easier for the reader to follow and understand the different aspects of achieving work-life balance.</t>
+  </si>
+  <si>
+    <t>Both results provide comprehensive answers to the query about achieving work-life balance, but they differ in structure and detail. Result_A is more structured, listing specific practices, strategies, tips, importance, and impact, along with relevant sources. This makes it easier to follow and understand. Result_B, while also detailed, is less structured and mixes different types of advice without clear categorization. This can make it slightly harder to follow. However, both results offer valuable insights and relevant sources. Result_A might be considered better due to its clearer structure and categorization, which enhances readability and comprehension.</t>
+  </si>
+  <si>
+    <t>Both results provide comprehensive answers to the query about achieving work-life balance, but they differ in structure and detail. Result_A is more structured, breaking down the information into specific categories and providing detailed explanations for each. It also includes direct links to relevant sources. Result_B, while also detailed, is less structured and more narrative in its approach. It provides practical tips but does not categorize them as clearly as Result_A. Result_A might be considered better for its structured approach and clear categorization, which can make it easier for readers to follow and understand. However, both results are good and provide valuable information.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -389,13 +383,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -403,6 +396,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -693,666 +716,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1656,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,19 +1095,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="6">
         <v>9</v>
@@ -1759,16 +1122,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4">
         <v>9</v>
@@ -1777,7 +1140,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -1786,19 +1149,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="4">
         <v>9</v>
@@ -1813,19 +1176,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4">
         <v>9</v>
@@ -1840,123 +1203,123 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E6" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F6" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
         <f>SUM(C2:C6)/5</f>
-        <v>6.4</v>
-      </c>
-      <c r="D7" s="8">
-        <f t="shared" ref="D7:H7" si="0">SUM(D2:D6)/5</f>
-        <v>6.6</v>
-      </c>
-      <c r="E7" s="8">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D7" s="4">
+        <f>SUM(D2:D6)/5</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E7" s="4">
+        <f>SUM(E2:E6)/5</f>
+        <v>9.4</v>
+      </c>
+      <c r="F7" s="4">
+        <f>SUM(F2:F6)/5</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G7" s="4">
+        <f>SUM(G2:G6)/5</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H7" s="4">
+        <f>SUM(H2:H6)/5</f>
+        <v>8.4</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4">
+        <f>C7-F7</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="D8" s="4">
+        <f>D7-G7</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <f>E7-H7</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <f>F7-C7</f>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:H8" si="0">G7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>6.6</v>
-      </c>
-      <c r="F7" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G7" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H7" s="8">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8">
-        <f>C7-F7</f>
-        <v>-2.5999999999999996</v>
-      </c>
-      <c r="D8" s="8">
-        <f>D7-G7</f>
-        <v>-2.4000000000000004</v>
-      </c>
-      <c r="E8" s="8">
-        <f>E7-H7</f>
-        <v>-1.8000000000000007</v>
-      </c>
-      <c r="F8" s="8">
-        <f>F7-C7</f>
-        <v>2.5999999999999996</v>
-      </c>
-      <c r="G8" s="8">
-        <f t="shared" ref="G8:H8" si="1">G7-D7</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="H8" s="8">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000007</v>
+        <v>-1</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9">
-        <v>8</v>
-      </c>
-      <c r="D9" s="9">
-        <v>9</v>
-      </c>
-      <c r="E9" s="9">
-        <v>8</v>
-      </c>
-      <c r="F9" s="9">
-        <v>7</v>
-      </c>
-      <c r="G9" s="9">
-        <v>6</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8">
+        <v>9</v>
+      </c>
+      <c r="E9" s="8">
+        <v>9</v>
+      </c>
+      <c r="F9" s="8">
+        <v>8</v>
+      </c>
+      <c r="G9" s="8">
+        <v>7</v>
+      </c>
+      <c r="H9" s="8">
         <v>7</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4">
         <v>8</v>
@@ -1968,10 +1331,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G10" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H10" s="4">
         <v>7</v>
@@ -1980,79 +1343,79 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F11" s="4">
         <v>7</v>
       </c>
       <c r="G11" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H11" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4">
         <v>8</v>
       </c>
       <c r="D12" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E12" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G12" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H12" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C13" s="7">
         <v>7</v>
       </c>
       <c r="D13" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="7">
         <v>8</v>
       </c>
       <c r="G13" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H13" s="7">
         <v>8</v>
@@ -2060,100 +1423,100 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
         <f>SUM(C9:C13)/5</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" ref="D14" si="1">SUM(D9:D13)/5</f>
+        <v>8.6</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" ref="E14" si="2">SUM(E9:E13)/5</f>
+        <v>8.4</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" ref="F14" si="3">SUM(F9:F13)/5</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" ref="G14" si="4">SUM(G9:G13)/5</f>
         <v>7.8</v>
       </c>
-      <c r="D14" s="8">
-        <f t="shared" ref="D14" si="2">SUM(D9:D13)/5</f>
+      <c r="H14" s="4">
+        <f t="shared" ref="H14" si="5">SUM(H9:H13)/5</f>
         <v>7.6</v>
       </c>
-      <c r="E14" s="8">
-        <f t="shared" ref="E14" si="3">SUM(E9:E13)/5</f>
-        <v>7.4</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" ref="F14" si="4">SUM(F9:F13)/5</f>
-        <v>7.2</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" ref="G14" si="5">SUM(G9:G13)/5</f>
-        <v>6.4</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" ref="H14" si="6">SUM(H9:H13)/5</f>
-        <v>6.8</v>
-      </c>
       <c r="I14" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
         <f>C14-F14</f>
-        <v>0.59999999999999964</v>
-      </c>
-      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
         <f>D14-G14</f>
-        <v>1.1999999999999993</v>
-      </c>
-      <c r="E15" s="8">
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="E15" s="4">
         <f>E14-H14</f>
-        <v>0.60000000000000053</v>
-      </c>
-      <c r="F15" s="8">
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="F15" s="4">
         <f>F14-C14</f>
-        <v>-0.59999999999999964</v>
-      </c>
-      <c r="G15" s="8">
-        <f t="shared" ref="G15" si="7">G14-D14</f>
-        <v>-1.1999999999999993</v>
-      </c>
-      <c r="H15" s="8">
-        <f t="shared" ref="H15" si="8">H14-E14</f>
-        <v>-0.60000000000000053</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" ref="G15" si="6">G14-D14</f>
+        <v>-0.79999999999999982</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" ref="H15" si="7">H14-E14</f>
+        <v>-0.80000000000000071</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="9">
-        <v>8</v>
-      </c>
-      <c r="D16" s="9">
-        <v>8</v>
-      </c>
-      <c r="E16" s="9">
-        <v>9</v>
-      </c>
-      <c r="F16" s="9">
-        <v>9</v>
-      </c>
-      <c r="G16" s="9">
-        <v>9</v>
-      </c>
-      <c r="H16" s="9">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="8">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8">
+        <v>9</v>
+      </c>
+      <c r="F16" s="8">
+        <v>8</v>
+      </c>
+      <c r="G16" s="8">
+        <v>8</v>
+      </c>
+      <c r="H16" s="8">
         <v>8</v>
       </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C17" s="4">
         <v>9</v>
@@ -2171,16 +1534,16 @@
         <v>8</v>
       </c>
       <c r="H17" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4">
         <v>9</v>
@@ -2198,16 +1561,16 @@
         <v>8</v>
       </c>
       <c r="H18" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C19" s="4">
         <v>9</v>
@@ -2225,16 +1588,16 @@
         <v>8</v>
       </c>
       <c r="H19" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C20" s="7">
         <v>9</v>
@@ -2243,7 +1606,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="7">
         <v>8</v>
@@ -2257,100 +1620,100 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4">
         <f>SUM(C16:C20)/5</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D21" s="8">
-        <f t="shared" ref="D21" si="9">SUM(D16:D20)/5</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E21" s="8">
-        <f t="shared" ref="E21" si="10">SUM(E16:E20)/5</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="F21" s="8">
-        <f t="shared" ref="F21" si="11">SUM(F16:F20)/5</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G21" s="8">
-        <f t="shared" ref="G21" si="12">SUM(G16:G20)/5</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H21" s="8">
-        <f t="shared" ref="H21" si="13">SUM(H16:H20)/5</f>
-        <v>7.6</v>
+        <v>9</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ref="D21" si="8">SUM(D16:D20)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" ref="E21" si="9">SUM(E16:E20)/5</f>
+        <v>9</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" ref="F21" si="10">SUM(F16:F20)/5</f>
+        <v>8</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" ref="G21" si="11">SUM(G16:G20)/5</f>
+        <v>8</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" ref="H21" si="12">SUM(H16:H20)/5</f>
+        <v>7.8</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4">
         <f>C21-F21</f>
-        <v>0.60000000000000142</v>
-      </c>
-      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
         <f>D21-G21</f>
-        <v>0.60000000000000142</v>
-      </c>
-      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
         <f>E21-H21</f>
-        <v>1.5999999999999996</v>
-      </c>
-      <c r="F22" s="8">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="F22" s="4">
         <f>F21-C21</f>
-        <v>-0.60000000000000142</v>
-      </c>
-      <c r="G22" s="8">
-        <f t="shared" ref="G22" si="14">G21-D21</f>
-        <v>-0.60000000000000142</v>
-      </c>
-      <c r="H22" s="8">
-        <f t="shared" ref="H22" si="15">H21-E21</f>
-        <v>-1.5999999999999996</v>
+        <v>-1</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" ref="G22" si="13">G21-D21</f>
+        <v>-1</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" ref="H22" si="14">H21-E21</f>
+        <v>-1.2000000000000002</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="9">
-        <v>9</v>
-      </c>
-      <c r="D23" s="9">
-        <v>9</v>
-      </c>
-      <c r="E23" s="9">
-        <v>9</v>
-      </c>
-      <c r="F23" s="9">
-        <v>7</v>
-      </c>
-      <c r="G23" s="9">
-        <v>7</v>
-      </c>
-      <c r="H23" s="9">
-        <v>6</v>
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="8">
+        <v>9</v>
+      </c>
+      <c r="D23" s="8">
+        <v>9</v>
+      </c>
+      <c r="E23" s="8">
+        <v>9</v>
+      </c>
+      <c r="F23" s="8">
+        <v>8</v>
+      </c>
+      <c r="G23" s="8">
+        <v>9</v>
+      </c>
+      <c r="H23" s="8">
+        <v>8</v>
       </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C24" s="4">
         <v>9</v>
@@ -2362,22 +1725,22 @@
         <v>9</v>
       </c>
       <c r="F24" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G24" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H24" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C25" s="4">
         <v>9</v>
@@ -2389,22 +1752,22 @@
         <v>9</v>
       </c>
       <c r="F25" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H25" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4">
         <v>9</v>
@@ -2416,192 +1779,192 @@
         <v>9</v>
       </c>
       <c r="F26" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H26" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="7">
+        <v>9</v>
+      </c>
+      <c r="D27" s="7">
+        <v>9</v>
+      </c>
+      <c r="E27" s="7">
+        <v>9</v>
+      </c>
+      <c r="F27" s="7">
+        <v>8</v>
+      </c>
+      <c r="G27" s="7">
+        <v>8</v>
+      </c>
+      <c r="H27" s="7">
+        <v>8</v>
+      </c>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4">
+        <f>SUM(C23:C27)/5</f>
+        <v>9</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ref="D28" si="15">SUM(D23:D27)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28" si="16">SUM(E23:E27)/5</f>
+        <v>9</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" ref="F28" si="17">SUM(F23:F27)/5</f>
+        <v>8</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" ref="G28" si="18">SUM(G23:G27)/5</f>
+        <v>8.6</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" ref="H28" si="19">SUM(H23:H27)/5</f>
+        <v>8</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="7">
-        <v>9</v>
-      </c>
-      <c r="D27" s="7">
-        <v>9</v>
-      </c>
-      <c r="E27" s="7">
-        <v>9</v>
-      </c>
-      <c r="F27" s="7">
-        <v>7</v>
-      </c>
-      <c r="G27" s="7">
-        <v>7</v>
-      </c>
-      <c r="H27" s="7">
-        <v>6</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8">
-        <f>SUM(C23:C27)/5</f>
-        <v>9</v>
-      </c>
-      <c r="D28" s="8">
-        <f t="shared" ref="D28" si="16">SUM(D23:D27)/5</f>
-        <v>9</v>
-      </c>
-      <c r="E28" s="8">
-        <f t="shared" ref="E28" si="17">SUM(E23:E27)/5</f>
-        <v>9</v>
-      </c>
-      <c r="F28" s="8">
-        <f t="shared" ref="F28" si="18">SUM(F23:F27)/5</f>
-        <v>7</v>
-      </c>
-      <c r="G28" s="8">
-        <f t="shared" ref="G28" si="19">SUM(G23:G27)/5</f>
-        <v>7.2</v>
-      </c>
-      <c r="H28" s="8">
-        <f t="shared" ref="H28" si="20">SUM(H23:H27)/5</f>
-        <v>6.2</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4">
         <f>C28-F28</f>
-        <v>2</v>
-      </c>
-      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
         <f>D28-G28</f>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="E29" s="8">
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E29" s="4">
         <f>E28-H28</f>
-        <v>2.8</v>
-      </c>
-      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
         <f>F28-C28</f>
-        <v>-2</v>
-      </c>
-      <c r="G29" s="8">
-        <f t="shared" ref="G29" si="21">G28-D28</f>
-        <v>-1.7999999999999998</v>
-      </c>
-      <c r="H29" s="8">
-        <f t="shared" ref="H29" si="22">H28-E28</f>
-        <v>-2.8</v>
+        <v>-1</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" ref="G29" si="20">G28-D28</f>
+        <v>-0.40000000000000036</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" ref="H29" si="21">H28-E28</f>
+        <v>-1</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="9">
-        <v>8</v>
-      </c>
-      <c r="D30" s="9">
-        <v>9</v>
-      </c>
-      <c r="E30" s="9">
-        <v>9</v>
-      </c>
-      <c r="F30" s="9">
-        <v>9</v>
-      </c>
-      <c r="G30" s="9">
-        <v>8</v>
-      </c>
-      <c r="H30" s="9">
-        <v>7</v>
+      <c r="A30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="8">
+        <v>9</v>
+      </c>
+      <c r="D30" s="8">
+        <v>8</v>
+      </c>
+      <c r="E30" s="8">
+        <v>7</v>
+      </c>
+      <c r="F30" s="8">
+        <v>7</v>
+      </c>
+      <c r="G30" s="8">
+        <v>9</v>
+      </c>
+      <c r="H30" s="8">
+        <v>9</v>
       </c>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4">
         <v>8</v>
       </c>
       <c r="D31" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F31" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G31" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H31" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C32" s="4">
         <v>8</v>
       </c>
       <c r="D32" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F32" s="4">
         <v>9</v>
       </c>
       <c r="G32" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H32" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C33" s="4">
         <v>8</v>
@@ -2610,156 +1973,156 @@
         <v>9</v>
       </c>
       <c r="E33" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="4">
         <v>9</v>
       </c>
       <c r="G33" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H33" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="7">
+        <v>8</v>
+      </c>
+      <c r="D34" s="7">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7">
+        <v>7</v>
+      </c>
+      <c r="F34" s="7">
+        <v>9</v>
+      </c>
+      <c r="G34" s="7">
+        <v>9</v>
+      </c>
+      <c r="H34" s="7">
+        <v>9</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4">
+        <f>SUM(C30:C34)/5</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" ref="D35" si="22">SUM(D30:D34)/5</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" ref="E35" si="23">SUM(E30:E34)/5</f>
+        <v>7.2</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" ref="F35" si="24">SUM(F30:F34)/5</f>
+        <v>8.6</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" ref="G35" si="25">SUM(G30:G34)/5</f>
+        <v>9</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" ref="H35" si="26">SUM(H30:H34)/5</f>
+        <v>9</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4">
+        <f>C35-F35</f>
+        <v>-0.40000000000000036</v>
+      </c>
+      <c r="D36" s="4">
+        <f>D35-G35</f>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="E36" s="4">
+        <f>E35-H35</f>
+        <v>-1.7999999999999998</v>
+      </c>
+      <c r="F36" s="4">
+        <f>F35-C35</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" ref="G36" si="27">G35-D35</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" ref="H36" si="28">H35-E35</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="7">
-        <v>7</v>
-      </c>
-      <c r="D34" s="7">
-        <v>8</v>
-      </c>
-      <c r="E34" s="7">
-        <v>7</v>
-      </c>
-      <c r="F34" s="7">
-        <v>9</v>
-      </c>
-      <c r="G34" s="7">
-        <v>9</v>
-      </c>
-      <c r="H34" s="7">
-        <v>8</v>
-      </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8">
-        <f>SUM(C30:C34)/5</f>
-        <v>7.8</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" ref="D35" si="23">SUM(D30:D34)/5</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E35" s="8">
-        <f t="shared" ref="E35" si="24">SUM(E30:E34)/5</f>
-        <v>8.6</v>
-      </c>
-      <c r="F35" s="8">
-        <f t="shared" ref="F35" si="25">SUM(F30:F34)/5</f>
-        <v>8.6</v>
-      </c>
-      <c r="G35" s="8">
-        <f t="shared" ref="G35" si="26">SUM(G30:G34)/5</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H35" s="8">
-        <f t="shared" ref="H35" si="27">SUM(H30:H34)/5</f>
-        <v>7.4</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8">
-        <f>C35-F35</f>
-        <v>-0.79999999999999982</v>
-      </c>
-      <c r="D36" s="8">
-        <f>D35-G35</f>
-        <v>0.60000000000000142</v>
-      </c>
-      <c r="E36" s="8">
-        <f>E35-H35</f>
-        <v>1.1999999999999993</v>
-      </c>
-      <c r="F36" s="8">
-        <f>F35-C35</f>
-        <v>0.79999999999999982</v>
-      </c>
-      <c r="G36" s="8">
-        <f t="shared" ref="G36" si="28">G35-D35</f>
-        <v>-0.60000000000000142</v>
-      </c>
-      <c r="H36" s="8">
-        <f t="shared" ref="H36" si="29">H35-E35</f>
-        <v>-1.1999999999999993</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="9">
-        <v>8</v>
-      </c>
-      <c r="D37" s="9">
-        <v>7</v>
-      </c>
-      <c r="E37" s="9">
-        <v>6</v>
-      </c>
-      <c r="F37" s="9">
-        <v>9</v>
-      </c>
-      <c r="G37" s="9">
-        <v>9</v>
-      </c>
-      <c r="H37" s="9">
+      <c r="A37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="8">
+        <v>9</v>
+      </c>
+      <c r="D37" s="8">
+        <v>9</v>
+      </c>
+      <c r="E37" s="8">
+        <v>10</v>
+      </c>
+      <c r="F37" s="8">
+        <v>8</v>
+      </c>
+      <c r="G37" s="8">
+        <v>8</v>
+      </c>
+      <c r="H37" s="8">
         <v>8</v>
       </c>
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C38" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D38" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E38" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F38" s="4">
         <v>8</v>
       </c>
       <c r="G38" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38" s="4">
         <v>8</v>
@@ -2768,52 +2131,52 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C39" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D39" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E39" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F39" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G39" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H39" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C40" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D40" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E40" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F40" s="4">
         <v>8</v>
       </c>
       <c r="G40" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H40" s="4">
         <v>8</v>
@@ -2822,25 +2185,25 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C41" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D41" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E41" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F41" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="7">
         <v>8</v>
@@ -2848,127 +2211,127 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4">
         <f>SUM(C37:C41)/5</f>
-        <v>7.2</v>
-      </c>
-      <c r="D42" s="8">
-        <f t="shared" ref="D42" si="30">SUM(D37:D41)/5</f>
-        <v>6.2</v>
-      </c>
-      <c r="E42" s="8">
-        <f t="shared" ref="E42" si="31">SUM(E37:E41)/5</f>
-        <v>6</v>
-      </c>
-      <c r="F42" s="8">
-        <f t="shared" ref="F42" si="32">SUM(F37:F41)/5</f>
-        <v>8.4</v>
-      </c>
-      <c r="G42" s="8">
-        <f t="shared" ref="G42" si="33">SUM(G37:G41)/5</f>
-        <v>9</v>
-      </c>
-      <c r="H42" s="8">
-        <f t="shared" ref="H42" si="34">SUM(H37:H41)/5</f>
-        <v>8.1999999999999993</v>
+        <v>9</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" ref="D42" si="29">SUM(D37:D41)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" ref="E42" si="30">SUM(E37:E41)/5</f>
+        <v>10</v>
+      </c>
+      <c r="F42" s="4">
+        <f t="shared" ref="F42" si="31">SUM(F37:F41)/5</f>
+        <v>7.6</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" ref="G42" si="32">SUM(G37:G41)/5</f>
+        <v>8</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" ref="H42" si="33">SUM(H37:H41)/5</f>
+        <v>8</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4">
         <f>C42-F42</f>
-        <v>-1.2000000000000002</v>
-      </c>
-      <c r="D43" s="8">
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="D43" s="4">
         <f>D42-G42</f>
-        <v>-2.8</v>
-      </c>
-      <c r="E43" s="8">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4">
         <f>E42-H42</f>
-        <v>-2.1999999999999993</v>
-      </c>
-      <c r="F43" s="8">
+        <v>2</v>
+      </c>
+      <c r="F43" s="4">
         <f>F42-C42</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="G43" s="8">
-        <f t="shared" ref="G43" si="35">G42-D42</f>
-        <v>2.8</v>
-      </c>
-      <c r="H43" s="8">
-        <f t="shared" ref="H43" si="36">H42-E42</f>
-        <v>2.1999999999999993</v>
+        <v>-1.4000000000000004</v>
+      </c>
+      <c r="G43" s="4">
+        <f t="shared" ref="G43" si="34">G42-D42</f>
+        <v>-1</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" ref="H43" si="35">H42-E42</f>
+        <v>-2</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="9">
-        <v>9</v>
-      </c>
-      <c r="D44" s="9">
-        <v>9</v>
-      </c>
-      <c r="E44" s="9">
-        <v>9</v>
-      </c>
-      <c r="F44" s="9">
-        <v>7</v>
-      </c>
-      <c r="G44" s="9">
-        <v>8</v>
-      </c>
-      <c r="H44" s="9">
-        <v>8</v>
+      <c r="A44" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="8">
+        <v>9</v>
+      </c>
+      <c r="D44" s="8">
+        <v>9</v>
+      </c>
+      <c r="E44" s="8">
+        <v>9</v>
+      </c>
+      <c r="F44" s="8">
+        <v>7</v>
+      </c>
+      <c r="G44" s="8">
+        <v>8</v>
+      </c>
+      <c r="H44" s="8">
+        <v>7</v>
       </c>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C45" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F45" s="4">
         <v>8</v>
       </c>
       <c r="G45" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C46" s="4">
         <v>9</v>
@@ -2992,10 +2355,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C47" s="4">
         <v>9</v>
@@ -3007,7 +2370,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="4">
         <v>8</v>
@@ -3019,22 +2382,22 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C48" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D48" s="7">
         <v>9</v>
       </c>
       <c r="E48" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G48" s="7">
         <v>8</v>
@@ -3045,100 +2408,100 @@
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4">
         <f>SUM(C44:C48)/5</f>
-        <v>8.4</v>
-      </c>
-      <c r="D49" s="8">
-        <f t="shared" ref="D49" si="37">SUM(D44:D48)/5</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E49" s="8">
-        <f t="shared" ref="E49" si="38">SUM(E44:E48)/5</f>
-        <v>8.4</v>
-      </c>
-      <c r="F49" s="8">
-        <f t="shared" ref="F49" si="39">SUM(F44:F48)/5</f>
-        <v>7.8</v>
-      </c>
-      <c r="G49" s="8">
-        <f t="shared" ref="G49" si="40">SUM(G44:G48)/5</f>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H49" s="8">
-        <f t="shared" ref="H49" si="41">SUM(H44:H48)/5</f>
-        <v>7.4</v>
+        <v>9</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" ref="D49" si="36">SUM(D44:D48)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" ref="E49" si="37">SUM(E44:E48)/5</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" ref="F49" si="38">SUM(F44:F48)/5</f>
+        <v>7.2</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" ref="G49" si="39">SUM(G44:G48)/5</f>
+        <v>8</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" ref="H49" si="40">SUM(H44:H48)/5</f>
+        <v>7</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4">
         <f>C49-F49</f>
-        <v>0.60000000000000053</v>
-      </c>
-      <c r="D50" s="8">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="D50" s="4">
         <f>D49-G49</f>
-        <v>0.60000000000000142</v>
-      </c>
-      <c r="E50" s="8">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
         <f>E49-H49</f>
-        <v>1</v>
-      </c>
-      <c r="F50" s="8">
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="F50" s="4">
         <f>F49-C49</f>
-        <v>-0.60000000000000053</v>
-      </c>
-      <c r="G50" s="8">
-        <f t="shared" ref="G50" si="42">G49-D49</f>
-        <v>-0.60000000000000142</v>
-      </c>
-      <c r="H50" s="8">
-        <f t="shared" ref="H50" si="43">H49-E49</f>
+        <v>-1.7999999999999998</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" ref="G50" si="41">G49-D49</f>
         <v>-1</v>
       </c>
+      <c r="H50" s="4">
+        <f t="shared" ref="H50" si="42">H49-E49</f>
+        <v>-2.1999999999999993</v>
+      </c>
       <c r="I50" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="9">
-        <v>9</v>
-      </c>
-      <c r="D51" s="9">
-        <v>9</v>
-      </c>
-      <c r="E51" s="9">
+      <c r="A51" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="8">
+        <v>9</v>
+      </c>
+      <c r="D51" s="8">
+        <v>9</v>
+      </c>
+      <c r="E51" s="8">
         <v>10</v>
       </c>
-      <c r="F51" s="9">
-        <v>8</v>
-      </c>
-      <c r="G51" s="9">
-        <v>7</v>
-      </c>
-      <c r="H51" s="9">
-        <v>7</v>
+      <c r="F51" s="8">
+        <v>7</v>
+      </c>
+      <c r="G51" s="8">
+        <v>7</v>
+      </c>
+      <c r="H51" s="8">
+        <v>6</v>
       </c>
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C52" s="4">
         <v>9</v>
@@ -3153,7 +2516,7 @@
         <v>8</v>
       </c>
       <c r="G52" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H52" s="4">
         <v>7</v>
@@ -3162,10 +2525,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C53" s="4">
         <v>9</v>
@@ -3183,16 +2546,16 @@
         <v>7</v>
       </c>
       <c r="H53" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C54" s="4">
         <v>9</v>
@@ -3204,22 +2567,22 @@
         <v>10</v>
       </c>
       <c r="F54" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H54" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C55" s="7">
         <v>9</v>
@@ -3234,7 +2597,7 @@
         <v>8</v>
       </c>
       <c r="G55" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H55" s="7">
         <v>7</v>
@@ -3242,100 +2605,100 @@
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4">
         <f>SUM(C51:C55)/5</f>
         <v>9</v>
       </c>
-      <c r="D56" s="8">
-        <f t="shared" ref="D56" si="44">SUM(D51:D55)/5</f>
-        <v>9</v>
-      </c>
-      <c r="E56" s="8">
-        <f t="shared" ref="E56" si="45">SUM(E51:E55)/5</f>
+      <c r="D56" s="4">
+        <f t="shared" ref="D56" si="43">SUM(D51:D55)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" ref="E56" si="44">SUM(E51:E55)/5</f>
         <v>10</v>
       </c>
-      <c r="F56" s="8">
-        <f t="shared" ref="F56" si="46">SUM(F51:F55)/5</f>
-        <v>8</v>
-      </c>
-      <c r="G56" s="8">
-        <f t="shared" ref="G56" si="47">SUM(G51:G55)/5</f>
-        <v>7.2</v>
-      </c>
-      <c r="H56" s="8">
-        <f t="shared" ref="H56" si="48">SUM(H51:H55)/5</f>
-        <v>7</v>
+      <c r="F56" s="4">
+        <f t="shared" ref="F56" si="45">SUM(F51:F55)/5</f>
+        <v>7.6</v>
+      </c>
+      <c r="G56" s="4">
+        <f t="shared" ref="G56" si="46">SUM(G51:G55)/5</f>
+        <v>7.4</v>
+      </c>
+      <c r="H56" s="4">
+        <f t="shared" ref="H56" si="47">SUM(H51:H55)/5</f>
+        <v>6.4</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4">
         <f>C56-F56</f>
-        <v>1</v>
-      </c>
-      <c r="D57" s="8">
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="D57" s="4">
         <f>D56-G56</f>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="E57" s="8">
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="E57" s="4">
         <f>E56-H56</f>
-        <v>3</v>
-      </c>
-      <c r="F57" s="8">
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="F57" s="4">
         <f>F56-C56</f>
-        <v>-1</v>
-      </c>
-      <c r="G57" s="8">
-        <f t="shared" ref="G57" si="49">G56-D56</f>
-        <v>-1.7999999999999998</v>
-      </c>
-      <c r="H57" s="8">
-        <f t="shared" ref="H57" si="50">H56-E56</f>
-        <v>-3</v>
+        <v>-1.4000000000000004</v>
+      </c>
+      <c r="G57" s="4">
+        <f t="shared" ref="G57" si="48">G56-D56</f>
+        <v>-1.5999999999999996</v>
+      </c>
+      <c r="H57" s="4">
+        <f t="shared" ref="H57" si="49">H56-E56</f>
+        <v>-3.5999999999999996</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="9">
-        <v>9</v>
-      </c>
-      <c r="D58" s="9">
-        <v>9</v>
-      </c>
-      <c r="E58" s="9">
-        <v>9</v>
-      </c>
-      <c r="F58" s="9">
-        <v>7</v>
-      </c>
-      <c r="G58" s="9">
-        <v>7</v>
-      </c>
-      <c r="H58" s="9">
-        <v>6</v>
+      <c r="A58" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="8">
+        <v>9</v>
+      </c>
+      <c r="D58" s="8">
+        <v>9</v>
+      </c>
+      <c r="E58" s="8">
+        <v>10</v>
+      </c>
+      <c r="F58" s="8">
+        <v>7</v>
+      </c>
+      <c r="G58" s="8">
+        <v>8</v>
+      </c>
+      <c r="H58" s="8">
+        <v>7</v>
       </c>
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C59" s="4">
         <v>9</v>
@@ -3344,13 +2707,13 @@
         <v>9</v>
       </c>
       <c r="E59" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F59" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H59" s="4">
         <v>7</v>
@@ -3359,25 +2722,25 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C60" s="4">
         <v>9</v>
       </c>
       <c r="D60" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" s="4">
         <v>9</v>
       </c>
       <c r="F60" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G60" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H60" s="4">
         <v>7</v>
@@ -3386,10 +2749,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C61" s="4">
         <v>9</v>
@@ -3398,25 +2761,25 @@
         <v>9</v>
       </c>
       <c r="E61" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F61" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G61" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C62" s="7">
         <v>9</v>
@@ -3425,13 +2788,13 @@
         <v>9</v>
       </c>
       <c r="E62" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F62" s="7">
         <v>7</v>
       </c>
       <c r="G62" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H62" s="7">
         <v>7</v>
@@ -3439,100 +2802,100 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4">
         <f>SUM(C58:C62)/5</f>
         <v>9</v>
       </c>
-      <c r="D63" s="8">
-        <f t="shared" ref="D63" si="51">SUM(D58:D62)/5</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="E63" s="8">
-        <f t="shared" ref="E63" si="52">SUM(E58:E62)/5</f>
-        <v>8.6</v>
-      </c>
-      <c r="F63" s="8">
-        <f t="shared" ref="F63" si="53">SUM(F58:F62)/5</f>
-        <v>7.6</v>
-      </c>
-      <c r="G63" s="8">
-        <f t="shared" ref="G63" si="54">SUM(G58:G62)/5</f>
-        <v>7</v>
-      </c>
-      <c r="H63" s="8">
-        <f t="shared" ref="H63" si="55">SUM(H58:H62)/5</f>
-        <v>6.6</v>
+      <c r="D63" s="4">
+        <f t="shared" ref="D63" si="50">SUM(D58:D62)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E63" s="4">
+        <f t="shared" ref="E63" si="51">SUM(E58:E62)/5</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F63" s="4">
+        <f t="shared" ref="F63" si="52">SUM(F58:F62)/5</f>
+        <v>7</v>
+      </c>
+      <c r="G63" s="4">
+        <f t="shared" ref="G63" si="53">SUM(G58:G62)/5</f>
+        <v>8</v>
+      </c>
+      <c r="H63" s="4">
+        <f t="shared" ref="H63" si="54">SUM(H58:H62)/5</f>
+        <v>7</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4">
         <f>C63-F63</f>
-        <v>1.4000000000000004</v>
-      </c>
-      <c r="D64" s="8">
+        <v>2</v>
+      </c>
+      <c r="D64" s="4">
         <f>D63-G63</f>
-        <v>2.1999999999999993</v>
-      </c>
-      <c r="E64" s="8">
+        <v>1</v>
+      </c>
+      <c r="E64" s="4">
         <f>E63-H63</f>
-        <v>2</v>
-      </c>
-      <c r="F64" s="8">
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="F64" s="4">
         <f>F63-C63</f>
-        <v>-1.4000000000000004</v>
-      </c>
-      <c r="G64" s="8">
-        <f t="shared" ref="G64" si="56">G63-D63</f>
-        <v>-2.1999999999999993</v>
-      </c>
-      <c r="H64" s="8">
-        <f t="shared" ref="H64" si="57">H63-E63</f>
         <v>-2</v>
       </c>
+      <c r="G64" s="4">
+        <f t="shared" ref="G64" si="55">G63-D63</f>
+        <v>-1</v>
+      </c>
+      <c r="H64" s="4">
+        <f t="shared" ref="H64" si="56">H63-E63</f>
+        <v>-2.8000000000000007</v>
+      </c>
       <c r="I64" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="9">
-        <v>9</v>
-      </c>
-      <c r="D65" s="9">
-        <v>9</v>
-      </c>
-      <c r="E65" s="9">
-        <v>10</v>
-      </c>
-      <c r="F65" s="9">
-        <v>8</v>
-      </c>
-      <c r="G65" s="9">
-        <v>8</v>
-      </c>
-      <c r="H65" s="9">
-        <v>7</v>
+      <c r="A65" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="8">
+        <v>9</v>
+      </c>
+      <c r="D65" s="8">
+        <v>9</v>
+      </c>
+      <c r="E65" s="8">
+        <v>9</v>
+      </c>
+      <c r="F65" s="8">
+        <v>8</v>
+      </c>
+      <c r="G65" s="8">
+        <v>8</v>
+      </c>
+      <c r="H65" s="8">
+        <v>8</v>
       </c>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C66" s="4">
         <v>9</v>
@@ -3541,7 +2904,7 @@
         <v>9</v>
       </c>
       <c r="E66" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" s="4">
         <v>8</v>
@@ -3550,16 +2913,16 @@
         <v>8</v>
       </c>
       <c r="H66" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C67" s="4">
         <v>9</v>
@@ -3568,25 +2931,25 @@
         <v>9</v>
       </c>
       <c r="E67" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G67" s="4">
         <v>8</v>
       </c>
       <c r="H67" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C68" s="4">
         <v>9</v>
@@ -3595,7 +2958,7 @@
         <v>9</v>
       </c>
       <c r="E68" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" s="4">
         <v>8</v>
@@ -3604,16 +2967,16 @@
         <v>8</v>
       </c>
       <c r="H68" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C69" s="7">
         <v>9</v>
@@ -3622,79 +2985,79 @@
         <v>9</v>
       </c>
       <c r="E69" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G69" s="7">
         <v>8</v>
       </c>
       <c r="H69" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="8">
+      <c r="C70" s="4">
         <f>SUM(C65:C69)/5</f>
         <v>9</v>
       </c>
-      <c r="D70" s="8">
-        <f t="shared" ref="D70" si="58">SUM(D65:D69)/5</f>
-        <v>9</v>
-      </c>
-      <c r="E70" s="8">
-        <f t="shared" ref="E70" si="59">SUM(E65:E69)/5</f>
-        <v>10</v>
-      </c>
-      <c r="F70" s="8">
-        <f t="shared" ref="F70" si="60">SUM(F65:F69)/5</f>
-        <v>8</v>
-      </c>
-      <c r="G70" s="8">
-        <f t="shared" ref="G70" si="61">SUM(G65:G69)/5</f>
-        <v>8</v>
-      </c>
-      <c r="H70" s="8">
-        <f t="shared" ref="H70" si="62">SUM(H65:H69)/5</f>
-        <v>7</v>
+      <c r="D70" s="4">
+        <f t="shared" ref="D70" si="57">SUM(D65:D69)/5</f>
+        <v>9</v>
+      </c>
+      <c r="E70" s="4">
+        <f t="shared" ref="E70" si="58">SUM(E65:E69)/5</f>
+        <v>9</v>
+      </c>
+      <c r="F70" s="4">
+        <f t="shared" ref="F70" si="59">SUM(F65:F69)/5</f>
+        <v>7.6</v>
+      </c>
+      <c r="G70" s="4">
+        <f t="shared" ref="G70" si="60">SUM(G65:G69)/5</f>
+        <v>8</v>
+      </c>
+      <c r="H70" s="4">
+        <f t="shared" ref="H70" si="61">SUM(H65:H69)/5</f>
+        <v>8</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="8">
+      <c r="C71" s="4">
         <f>C70-F70</f>
-        <v>1</v>
-      </c>
-      <c r="D71" s="8">
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="D71" s="4">
         <f>D70-G70</f>
         <v>1</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="4">
         <f>E70-H70</f>
-        <v>3</v>
-      </c>
-      <c r="F71" s="8">
+        <v>1</v>
+      </c>
+      <c r="F71" s="4">
         <f>F70-C70</f>
+        <v>-1.4000000000000004</v>
+      </c>
+      <c r="G71" s="4">
+        <f t="shared" ref="G71" si="62">G70-D70</f>
         <v>-1</v>
       </c>
-      <c r="G71" s="8">
-        <f t="shared" ref="G71" si="63">G70-D70</f>
+      <c r="H71" s="4">
+        <f t="shared" ref="H71" si="63">H70-E70</f>
         <v>-1</v>
       </c>
-      <c r="H71" s="8">
-        <f t="shared" ref="H71" si="64">H70-E70</f>
-        <v>-3</v>
-      </c>
       <c r="I71" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3724,30 +3087,30 @@
       <c r="B74" s="4"/>
       <c r="C74" s="4">
         <f>C29+C36+C43+C50+C57+C64+C71</f>
-        <v>4.0000000000000009</v>
+        <v>8.6000000000000014</v>
       </c>
       <c r="D74" s="4">
-        <f t="shared" ref="D74:H74" si="65">D29+D36+D43+D50+D57+D64+D71</f>
-        <v>5.200000000000002</v>
+        <f t="shared" ref="D74:H74" si="64">D29+D36+D43+D50+D57+D64+D71</f>
+        <v>5.1999999999999993</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="65"/>
+        <f t="shared" si="64"/>
         <v>10.8</v>
       </c>
       <c r="F74" s="4">
-        <f t="shared" si="65"/>
-        <v>-4.0000000000000009</v>
+        <f t="shared" si="64"/>
+        <v>-8.6000000000000014</v>
       </c>
       <c r="G74" s="4">
-        <f t="shared" si="65"/>
-        <v>-5.200000000000002</v>
+        <f t="shared" si="64"/>
+        <v>-5.1999999999999993</v>
       </c>
       <c r="H74" s="4">
-        <f t="shared" si="65"/>
+        <f t="shared" si="64"/>
         <v>-10.8</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4115,120 +3478,125 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8:H8">
-    <cfRule type="cellIs" dxfId="62" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:H15">
-    <cfRule type="cellIs" dxfId="59" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:H22">
-    <cfRule type="cellIs" dxfId="56" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:H29">
-    <cfRule type="cellIs" dxfId="53" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:H36">
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:H43">
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:H50">
-    <cfRule type="cellIs" dxfId="44" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:H57">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:H64">
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:H71">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:H74">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:E8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4247,48 +3615,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>7.8</v>
@@ -4329,7 +3697,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>8.8000000000000007</v>
@@ -4370,7 +3738,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>7.8</v>
@@ -4411,7 +3779,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>8.4</v>
@@ -4452,7 +3820,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -4493,7 +3861,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -4534,7 +3902,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>7.2</v>
@@ -4575,7 +3943,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -4657,7 +4025,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>9</v>

</xml_diff>